<commit_message>
Fix error in the add_chart function
- Fix error: E2.
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -1,3 +1,98 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
+</workbook>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt formatCode="[$$-C09]#,##0.00;[RED]\-[$$-C09]#,##0.00" numFmtId="164"/>
+  </numFmts>
+  <fonts count="4">
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="6">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="5">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+  </cellXfs>
+  <cellStyles count="6">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
+  </cellStyles>
+</styleSheet>
+</file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
@@ -283,7 +378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -370,6 +465,5 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>